<commit_message>
jos korpaaa i dumrem
</commit_message>
<xml_diff>
--- a/ApotekaGUI/podaci.xlsx
+++ b/ApotekaGUI/podaci.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="131">
   <si>
     <t>NAZIV</t>
   </si>
@@ -352,19 +352,40 @@
     <t>Vujic</t>
   </si>
   <si>
-    <t>LEKAR</t>
-  </si>
-  <si>
-    <t>JMBGPACIJENTA</t>
+    <t>IDENTIF. LEKARA</t>
+  </si>
+  <si>
+    <t>JMBG PACIJENTA</t>
   </si>
   <si>
     <t>DATUM I VREME</t>
   </si>
   <si>
+    <t>LEK</t>
+  </si>
+  <si>
+    <t>KOLICINA</t>
+  </si>
+  <si>
+    <t>UKUPNA CENA</t>
+  </si>
+  <si>
+    <t>10.8.2020 14:40</t>
+  </si>
+  <si>
+    <t>11.8.2020 14:40</t>
+  </si>
+  <si>
+    <t>12.8.2020 14:40</t>
+  </si>
+  <si>
+    <t>13.8.2020 14:40</t>
+  </si>
+  <si>
+    <t>14.8.2020 14:40</t>
+  </si>
+  <si>
     <t>PRODAVAC</t>
-  </si>
-  <si>
-    <t>KOLICINA</t>
   </si>
   <si>
     <t>UKUPNA ZARADA</t>
@@ -402,15 +423,16 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <sz val="9.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -426,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -436,19 +458,20 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -708,7 +731,7 @@
       <c r="B2" s="1">
         <v>121212.0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -725,7 +748,7 @@
       <c r="B3" s="1">
         <v>131313.0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -742,7 +765,7 @@
       <c r="B4" s="1">
         <v>141414.0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -759,7 +782,7 @@
       <c r="B5" s="1">
         <v>151515.0</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -776,10 +799,10 @@
       <c r="B6" s="1">
         <v>161616.0</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="1">
@@ -793,7 +816,7 @@
       <c r="B7" s="1">
         <v>171717.0</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -810,7 +833,7 @@
       <c r="B8" s="1">
         <v>181818.0</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -827,7 +850,7 @@
       <c r="B9" s="1">
         <v>191919.0</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -844,7 +867,7 @@
       <c r="B10" s="1">
         <v>202020.0</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -861,7 +884,7 @@
       <c r="B11" s="1">
         <v>212121.0</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -878,7 +901,7 @@
       <c r="B12" s="1">
         <v>222222.0</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -895,13 +918,13 @@
       <c r="B13" s="1">
         <v>232323.0</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>279.0</v>
       </c>
     </row>
@@ -912,7 +935,7 @@
       <c r="B14" s="1">
         <v>242424.0</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -929,13 +952,13 @@
       <c r="B15" s="1">
         <v>252525.0</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>100.0</v>
       </c>
     </row>
@@ -946,7 +969,7 @@
       <c r="B16" s="1">
         <v>262626.0</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -963,13 +986,13 @@
       <c r="B17" s="1">
         <v>272727.0</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>759.0</v>
       </c>
     </row>
@@ -980,7 +1003,7 @@
       <c r="B18" s="1">
         <v>282828.0</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -997,13 +1020,13 @@
       <c r="B19" s="1">
         <v>292929.0</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <v>79.0</v>
       </c>
     </row>
@@ -1014,7 +1037,7 @@
       <c r="B20" s="1">
         <v>303030.0</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1031,13 +1054,13 @@
       <c r="B21" s="1">
         <v>313131.0</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>299.0</v>
       </c>
     </row>
@@ -1048,7 +1071,7 @@
       <c r="B22" s="1">
         <v>323232.0</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -1065,7 +1088,7 @@
       <c r="B23" s="1">
         <v>333333.0</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1082,7 +1105,7 @@
       <c r="B24" s="1">
         <v>343434.0</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -1099,7 +1122,7 @@
       <c r="B25" s="1">
         <v>353535.0</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1116,13 +1139,13 @@
       <c r="B26" s="1">
         <v>363636.0</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="1">
         <v>199.0</v>
       </c>
     </row>
@@ -1133,7 +1156,7 @@
       <c r="B27" s="1">
         <v>373737.0</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1150,7 +1173,7 @@
       <c r="B28" s="1">
         <v>383838.0</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1167,7 +1190,7 @@
       <c r="B29" s="1">
         <v>393939.0</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1184,7 +1207,7 @@
       <c r="B30" s="1">
         <v>404040.0</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -1201,7 +1224,7 @@
       <c r="B31" s="1">
         <v>414141.0</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1218,7 +1241,7 @@
       <c r="B32" s="1">
         <v>424242.0</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1235,7 +1258,7 @@
       <c r="B33" s="1">
         <v>434343.0</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -1252,7 +1275,7 @@
       <c r="B34" s="1">
         <v>444444.0</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1269,7 +1292,7 @@
       <c r="B35" s="1">
         <v>454545.0</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1367,155 +1390,155 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1534,6 +1557,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="2" max="2" width="17.0"/>
     <col customWidth="1" min="3" max="3" width="19.71"/>
     <col customWidth="1" min="4" max="4" width="20.0"/>
   </cols>
@@ -1550,6 +1574,153 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>114</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>121212.0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.505995455033E12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>200.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3">
+        <v>131313.0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.606955632544E12</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1000.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3">
+        <v>141414.0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.101991865033E12</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>2400.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3">
+        <v>151515.0</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1.808988412355E12</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1400.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>161616.0</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.510945563288E12</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2245.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>171717.0</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2.101002645899E12</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2100.0</v>
       </c>
     </row>
   </sheetData>
@@ -1583,17 +1754,17 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>117</v>
+      <c r="F1" s="7" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1">
@@ -1603,17 +1774,17 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E2" s="2">
+        <v>125</v>
+      </c>
+      <c r="E2" s="1">
         <v>1.0</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="8">
         <v>200.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1">
@@ -1623,17 +1794,17 @@
         <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E3" s="2">
+        <v>126</v>
+      </c>
+      <c r="E3" s="1">
         <v>2.0</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="8">
         <v>1000.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1">
@@ -1643,17 +1814,17 @@
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E4" s="2">
+        <v>127</v>
+      </c>
+      <c r="E4" s="1">
         <v>3.0</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="8">
         <v>2400.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="1">
@@ -1663,17 +1834,17 @@
         <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E5" s="2">
+        <v>128</v>
+      </c>
+      <c r="E5" s="1">
         <v>4.0</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="8">
         <v>1400.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="1">
@@ -1683,12 +1854,12 @@
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" s="2">
+        <v>129</v>
+      </c>
+      <c r="E6" s="1">
         <v>5.0</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="8">
         <v>2245.0</v>
       </c>
     </row>
@@ -1703,17 +1874,17 @@
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="2">
+        <v>130</v>
+      </c>
+      <c r="E7" s="1">
         <v>6.0</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="8">
         <v>2100.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="F8" s="7"/>
+      <c r="F8" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>